<commit_message>
initial commit for release version
</commit_message>
<xml_diff>
--- a/Project_Sheet.xlsx
+++ b/Project_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\majoron\Python\project\project-time-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253D6CD8-4A81-4D79-ACA6-9CBC29473505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CBAD3-7710-4E89-9FC7-14DBF3C8BCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="1890" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listopad2023" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -432,12 +432,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -514,7 +545,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -782,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL37"/>
+  <dimension ref="A1:BL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +885,7 @@
       <c r="AW1" s="3"/>
       <c r="AX1" s="4"/>
     </row>
-    <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -908,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36"/>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
@@ -958,7 +995,7 @@
       <c r="AU3" s="11"/>
       <c r="AV3" s="11"/>
       <c r="AW3" s="11">
-        <f t="shared" ref="AW3:AW33" si="0">SUM(C3:AV3)</f>
+        <f t="shared" ref="AW3:AW37" si="0">SUM(C3:AV3)</f>
         <v>0</v>
       </c>
       <c r="AX3" s="12">
@@ -980,8 +1017,8 @@
       <c r="BK3" s="13"/>
       <c r="BL3" s="13"/>
     </row>
-    <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+    <row r="4" spans="1:64" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="37"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -1038,8 +1075,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+    <row r="5" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="37"/>
       <c r="B5" s="15"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1096,8 +1133,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+    <row r="6" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37"/>
       <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
@@ -1156,8 +1193,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
+    <row r="7" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="37"/>
       <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
@@ -1216,8 +1253,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
+    <row r="8" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="37"/>
       <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
@@ -1276,8 +1313,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+    <row r="9" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="37"/>
       <c r="B9" s="10"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -1348,85 +1385,77 @@
       <c r="BK9" s="13"/>
       <c r="BL9" s="13"/>
     </row>
-    <row r="10" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="1:64" s="13" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="37"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
+      <c r="AL10" s="25"/>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="25"/>
+      <c r="AO10" s="25"/>
+      <c r="AP10" s="25"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="25"/>
+      <c r="AS10" s="25"/>
+      <c r="AT10" s="25"/>
+      <c r="AU10" s="25"/>
+      <c r="AV10" s="25"/>
+      <c r="AW10" s="26"/>
+      <c r="AX10" s="12"/>
+    </row>
+    <row r="11" spans="1:64" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="37"/>
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="18"/>
-      <c r="AH10" s="18"/>
-      <c r="AI10" s="18"/>
-      <c r="AJ10" s="18"/>
-      <c r="AK10" s="18"/>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="18"/>
-      <c r="AN10" s="18"/>
-      <c r="AO10" s="18"/>
-      <c r="AP10" s="18"/>
-      <c r="AQ10" s="18"/>
-      <c r="AR10" s="18"/>
-      <c r="AS10" s="18"/>
-      <c r="AT10" s="18"/>
-      <c r="AU10" s="24"/>
-      <c r="AV10" s="24"/>
-      <c r="AW10" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX10" s="21">
-        <f>IF(AW10&gt;7.5, AW10 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
@@ -1457,8 +1486,8 @@
       <c r="AR11" s="18"/>
       <c r="AS11" s="18"/>
       <c r="AT11" s="18"/>
-      <c r="AU11" s="18"/>
-      <c r="AV11" s="18"/>
+      <c r="AU11" s="24"/>
+      <c r="AV11" s="24"/>
       <c r="AW11" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1468,19 +1497,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="37"/>
       <c r="B12" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
@@ -1517,7 +1546,7 @@
       <c r="AR12" s="18"/>
       <c r="AS12" s="18"/>
       <c r="AT12" s="18"/>
-      <c r="AU12" s="24"/>
+      <c r="AU12" s="18"/>
       <c r="AV12" s="18"/>
       <c r="AW12" s="20">
         <f t="shared" si="0"/>
@@ -1528,18 +1557,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+    <row r="13" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="37"/>
       <c r="B13" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="18"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="18"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
@@ -1588,12 +1617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+    <row r="14" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="37"/>
       <c r="B14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="16"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -1629,7 +1658,7 @@
       <c r="AJ14" s="18"/>
       <c r="AK14" s="18"/>
       <c r="AL14" s="18"/>
-      <c r="AM14" s="19"/>
+      <c r="AM14" s="18"/>
       <c r="AN14" s="18"/>
       <c r="AO14" s="18"/>
       <c r="AP14" s="18"/>
@@ -1637,7 +1666,7 @@
       <c r="AR14" s="18"/>
       <c r="AS14" s="18"/>
       <c r="AT14" s="18"/>
-      <c r="AU14" s="18"/>
+      <c r="AU14" s="24"/>
       <c r="AV14" s="18"/>
       <c r="AW14" s="20">
         <f t="shared" si="0"/>
@@ -1648,202 +1677,194 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="25"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
-      <c r="AI15" s="25"/>
-      <c r="AJ15" s="25"/>
-      <c r="AK15" s="25"/>
-      <c r="AL15" s="25"/>
-      <c r="AM15" s="25"/>
-      <c r="AN15" s="25"/>
-      <c r="AO15" s="25"/>
-      <c r="AP15" s="25"/>
-      <c r="AQ15" s="25"/>
-      <c r="AR15" s="25"/>
-      <c r="AS15" s="25"/>
-      <c r="AT15" s="25"/>
-      <c r="AU15" s="25"/>
-      <c r="AV15" s="25"/>
-      <c r="AW15" s="26">
+    <row r="15" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37"/>
+      <c r="B15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="18"/>
+      <c r="AM15" s="19"/>
+      <c r="AN15" s="18"/>
+      <c r="AO15" s="18"/>
+      <c r="AP15" s="18"/>
+      <c r="AQ15" s="18"/>
+      <c r="AR15" s="18"/>
+      <c r="AS15" s="18"/>
+      <c r="AT15" s="18"/>
+      <c r="AU15" s="18"/>
+      <c r="AV15" s="18"/>
+      <c r="AW15" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX15" s="12">
-        <f>IF(AW15&gt;0, AW15, )</f>
-        <v>0</v>
-      </c>
-      <c r="AY15" s="13"/>
-      <c r="AZ15" s="13"/>
-      <c r="BA15" s="13"/>
-      <c r="BB15" s="13"/>
-      <c r="BC15" s="13"/>
-      <c r="BD15" s="13"/>
-      <c r="BE15" s="13"/>
-      <c r="BF15" s="13"/>
-      <c r="BG15" s="13"/>
-      <c r="BH15" s="13"/>
-      <c r="BI15" s="13"/>
-      <c r="BJ15" s="13"/>
-      <c r="BK15" s="13"/>
-      <c r="BL15" s="13"/>
-    </row>
-    <row r="16" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="15" t="s">
+      <c r="AX15" s="21">
+        <f>IF(AW15&gt;7.5, AW15 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="37"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="25"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+      <c r="AG16" s="25"/>
+      <c r="AH16" s="25"/>
+      <c r="AI16" s="25"/>
+      <c r="AJ16" s="25"/>
+      <c r="AK16" s="25"/>
+      <c r="AL16" s="25"/>
+      <c r="AM16" s="25"/>
+      <c r="AN16" s="25"/>
+      <c r="AO16" s="25"/>
+      <c r="AP16" s="25"/>
+      <c r="AQ16" s="25"/>
+      <c r="AR16" s="25"/>
+      <c r="AS16" s="25"/>
+      <c r="AT16" s="25"/>
+      <c r="AU16" s="25"/>
+      <c r="AV16" s="25"/>
+      <c r="AW16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX16" s="12">
+        <f>IF(AW16&gt;0, AW16, )</f>
+        <v>0</v>
+      </c>
+      <c r="AY16" s="13"/>
+      <c r="AZ16" s="13"/>
+      <c r="BA16" s="13"/>
+      <c r="BB16" s="13"/>
+      <c r="BC16" s="13"/>
+      <c r="BD16" s="13"/>
+      <c r="BE16" s="13"/>
+      <c r="BF16" s="13"/>
+      <c r="BG16" s="13"/>
+      <c r="BH16" s="13"/>
+      <c r="BI16" s="13"/>
+      <c r="BJ16" s="13"/>
+      <c r="BK16" s="13"/>
+      <c r="BL16" s="13"/>
+    </row>
+    <row r="17" spans="1:64" s="13" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="37"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="25"/>
+      <c r="AD17" s="25"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AJ17" s="25"/>
+      <c r="AK17" s="25"/>
+      <c r="AL17" s="25"/>
+      <c r="AM17" s="25"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
+      <c r="AQ17" s="25"/>
+      <c r="AR17" s="25"/>
+      <c r="AS17" s="25"/>
+      <c r="AT17" s="25"/>
+      <c r="AU17" s="25"/>
+      <c r="AV17" s="25"/>
+      <c r="AW17" s="26"/>
+      <c r="AX17" s="12"/>
+    </row>
+    <row r="18" spans="1:64" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="37"/>
+      <c r="B18" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
-      <c r="AJ16" s="18"/>
-      <c r="AK16" s="18"/>
-      <c r="AL16" s="18"/>
-      <c r="AM16" s="18"/>
-      <c r="AN16" s="18"/>
-      <c r="AO16" s="18"/>
-      <c r="AP16" s="18"/>
-      <c r="AQ16" s="18"/>
-      <c r="AR16" s="18"/>
-      <c r="AS16" s="18"/>
-      <c r="AT16" s="18"/>
-      <c r="AU16" s="18"/>
-      <c r="AV16" s="18"/>
-      <c r="AW16" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX16" s="21">
-        <f>IF(AW16&gt;7.5, AW16 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="18"/>
-      <c r="AJ17" s="18"/>
-      <c r="AK17" s="18"/>
-      <c r="AL17" s="18"/>
-      <c r="AM17" s="18"/>
-      <c r="AN17" s="18"/>
-      <c r="AO17" s="18"/>
-      <c r="AP17" s="18"/>
-      <c r="AQ17" s="18"/>
-      <c r="AR17" s="18"/>
-      <c r="AS17" s="18"/>
-      <c r="AT17" s="18"/>
-      <c r="AU17" s="18"/>
-      <c r="AV17" s="18"/>
-      <c r="AW17" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX17" s="21">
-        <f>IF(AW17&gt;7.5, AW17 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -1900,10 +1921,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="37"/>
       <c r="B19" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -1960,10 +1981,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="37"/>
       <c r="B20" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -2020,84 +2041,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="25"/>
-      <c r="AE21" s="25"/>
-      <c r="AF21" s="25"/>
-      <c r="AG21" s="25"/>
-      <c r="AH21" s="25"/>
-      <c r="AI21" s="25"/>
-      <c r="AJ21" s="25"/>
-      <c r="AK21" s="25"/>
-      <c r="AL21" s="25"/>
-      <c r="AM21" s="25"/>
-      <c r="AN21" s="25"/>
-      <c r="AO21" s="25"/>
-      <c r="AP21" s="25"/>
-      <c r="AQ21" s="25"/>
-      <c r="AR21" s="25"/>
-      <c r="AS21" s="25"/>
-      <c r="AT21" s="25"/>
-      <c r="AU21" s="25"/>
-      <c r="AV21" s="25"/>
-      <c r="AW21" s="26">
+    <row r="21" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="37"/>
+      <c r="B21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
+      <c r="AH21" s="18"/>
+      <c r="AI21" s="18"/>
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="18"/>
+      <c r="AM21" s="18"/>
+      <c r="AN21" s="18"/>
+      <c r="AO21" s="18"/>
+      <c r="AP21" s="18"/>
+      <c r="AQ21" s="18"/>
+      <c r="AR21" s="18"/>
+      <c r="AS21" s="18"/>
+      <c r="AT21" s="18"/>
+      <c r="AU21" s="18"/>
+      <c r="AV21" s="18"/>
+      <c r="AW21" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX21" s="12">
-        <f>IF(AW21&gt;0, AW21, )</f>
-        <v>0</v>
-      </c>
-      <c r="AY21" s="13"/>
-      <c r="AZ21" s="13"/>
-      <c r="BA21" s="13"/>
-      <c r="BB21" s="13"/>
-      <c r="BC21" s="13"/>
-      <c r="BD21" s="13"/>
-      <c r="BE21" s="13"/>
-      <c r="BF21" s="13"/>
-      <c r="BG21" s="13"/>
-      <c r="BH21" s="13"/>
-      <c r="BI21" s="13"/>
-      <c r="BJ21" s="13"/>
-      <c r="BK21" s="13"/>
-      <c r="BL21" s="13"/>
-    </row>
-    <row r="22" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+      <c r="AX21" s="21">
+        <f>IF(AW21&gt;7.5, AW21 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37"/>
       <c r="B22" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="27"/>
+        <v>17</v>
+      </c>
+      <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
@@ -2152,130 +2161,134 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="18"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="18"/>
-      <c r="AJ23" s="18"/>
-      <c r="AK23" s="18"/>
-      <c r="AL23" s="18"/>
-      <c r="AM23" s="18"/>
-      <c r="AN23" s="18"/>
-      <c r="AO23" s="18"/>
-      <c r="AP23" s="18"/>
-      <c r="AQ23" s="18"/>
-      <c r="AR23" s="18"/>
-      <c r="AS23" s="18"/>
-      <c r="AT23" s="18"/>
-      <c r="AU23" s="18"/>
-      <c r="AV23" s="18"/>
-      <c r="AW23" s="20">
+    <row r="23" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="37"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
+      <c r="AA23" s="25"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="25"/>
+      <c r="AD23" s="25"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
+      <c r="AI23" s="25"/>
+      <c r="AJ23" s="25"/>
+      <c r="AK23" s="25"/>
+      <c r="AL23" s="25"/>
+      <c r="AM23" s="25"/>
+      <c r="AN23" s="25"/>
+      <c r="AO23" s="25"/>
+      <c r="AP23" s="25"/>
+      <c r="AQ23" s="25"/>
+      <c r="AR23" s="25"/>
+      <c r="AS23" s="25"/>
+      <c r="AT23" s="25"/>
+      <c r="AU23" s="25"/>
+      <c r="AV23" s="25"/>
+      <c r="AW23" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX23" s="21">
-        <f>IF(AW23&gt;7.5, AW23 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="18"/>
-      <c r="AA24" s="18"/>
-      <c r="AB24" s="18"/>
-      <c r="AC24" s="18"/>
-      <c r="AD24" s="18"/>
-      <c r="AE24" s="18"/>
-      <c r="AF24" s="18"/>
-      <c r="AG24" s="18"/>
-      <c r="AH24" s="18"/>
-      <c r="AI24" s="18"/>
-      <c r="AJ24" s="18"/>
-      <c r="AK24" s="18"/>
-      <c r="AL24" s="18"/>
-      <c r="AM24" s="18"/>
-      <c r="AN24" s="18"/>
-      <c r="AO24" s="18"/>
-      <c r="AP24" s="18"/>
-      <c r="AQ24" s="18"/>
-      <c r="AR24" s="18"/>
-      <c r="AS24" s="18"/>
-      <c r="AT24" s="18"/>
-      <c r="AU24" s="18"/>
-      <c r="AV24" s="18"/>
-      <c r="AW24" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX24" s="21">
-        <f>IF(AW24&gt;7.5, AW24 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+      <c r="AX23" s="12">
+        <f>IF(AW23&gt;0, AW23, )</f>
+        <v>0</v>
+      </c>
+      <c r="AY23" s="13"/>
+      <c r="AZ23" s="13"/>
+      <c r="BA23" s="13"/>
+      <c r="BB23" s="13"/>
+      <c r="BC23" s="13"/>
+      <c r="BD23" s="13"/>
+      <c r="BE23" s="13"/>
+      <c r="BF23" s="13"/>
+      <c r="BG23" s="13"/>
+      <c r="BH23" s="13"/>
+      <c r="BI23" s="13"/>
+      <c r="BJ23" s="13"/>
+      <c r="BK23" s="13"/>
+      <c r="BL23" s="13"/>
+    </row>
+    <row r="24" spans="1:64" s="13" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="25"/>
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
+      <c r="AH24" s="25"/>
+      <c r="AI24" s="25"/>
+      <c r="AJ24" s="25"/>
+      <c r="AK24" s="25"/>
+      <c r="AL24" s="25"/>
+      <c r="AM24" s="25"/>
+      <c r="AN24" s="25"/>
+      <c r="AO24" s="25"/>
+      <c r="AP24" s="25"/>
+      <c r="AQ24" s="25"/>
+      <c r="AR24" s="25"/>
+      <c r="AS24" s="25"/>
+      <c r="AT24" s="25"/>
+      <c r="AU24" s="25"/>
+      <c r="AV24" s="25"/>
+      <c r="AW24" s="26"/>
+      <c r="AX24" s="12"/>
+    </row>
+    <row r="25" spans="1:64" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="37"/>
       <c r="B25" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C25" s="27"/>
       <c r="D25" s="18"/>
@@ -2332,10 +2345,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="37"/>
       <c r="B26" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="18"/>
@@ -2392,91 +2405,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="25"/>
-      <c r="AE27" s="25"/>
-      <c r="AF27" s="25"/>
-      <c r="AG27" s="25"/>
-      <c r="AH27" s="25"/>
-      <c r="AI27" s="25"/>
-      <c r="AJ27" s="25"/>
-      <c r="AK27" s="25"/>
-      <c r="AL27" s="25"/>
-      <c r="AM27" s="25"/>
-      <c r="AN27" s="25"/>
-      <c r="AO27" s="25"/>
-      <c r="AP27" s="25"/>
-      <c r="AQ27" s="25"/>
-      <c r="AR27" s="25"/>
-      <c r="AS27" s="25"/>
-      <c r="AT27" s="25"/>
-      <c r="AU27" s="25"/>
-      <c r="AV27" s="25"/>
-      <c r="AW27" s="26">
+    <row r="27" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="37"/>
+      <c r="B27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+      <c r="AA27" s="18"/>
+      <c r="AB27" s="18"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="18"/>
+      <c r="AE27" s="18"/>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="18"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="18"/>
+      <c r="AM27" s="18"/>
+      <c r="AN27" s="18"/>
+      <c r="AO27" s="18"/>
+      <c r="AP27" s="18"/>
+      <c r="AQ27" s="18"/>
+      <c r="AR27" s="18"/>
+      <c r="AS27" s="18"/>
+      <c r="AT27" s="18"/>
+      <c r="AU27" s="18"/>
+      <c r="AV27" s="18"/>
+      <c r="AW27" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX27" s="12">
-        <f>IF(AW27&gt;0, AW27, )</f>
-        <v>0</v>
-      </c>
-      <c r="AY27" s="13"/>
-      <c r="AZ27" s="13"/>
-      <c r="BA27" s="13"/>
-      <c r="BB27" s="13"/>
-      <c r="BC27" s="13"/>
-      <c r="BD27" s="13"/>
-      <c r="BE27" s="13"/>
-      <c r="BF27" s="13"/>
-      <c r="BG27" s="13"/>
-      <c r="BH27" s="13"/>
-      <c r="BI27" s="13"/>
-      <c r="BJ27" s="13"/>
-      <c r="BK27" s="13"/>
-      <c r="BL27" s="13"/>
-    </row>
-    <row r="28" spans="1:64" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
+      <c r="AX27" s="21">
+        <f>IF(AW27&gt;7.5, AW27 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="37"/>
       <c r="B28" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
@@ -2484,11 +2485,11 @@
       <c r="O28" s="18"/>
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
       <c r="W28" s="18"/>
       <c r="X28" s="18"/>
       <c r="Y28" s="18"/>
@@ -2497,18 +2498,18 @@
       <c r="AB28" s="18"/>
       <c r="AC28" s="18"/>
       <c r="AD28" s="18"/>
-      <c r="AE28" s="27"/>
-      <c r="AF28" s="27"/>
-      <c r="AG28" s="27"/>
-      <c r="AH28" s="27"/>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="27"/>
-      <c r="AK28" s="27"/>
-      <c r="AL28" s="27"/>
-      <c r="AM28" s="27"/>
-      <c r="AN28" s="27"/>
-      <c r="AO28" s="27"/>
-      <c r="AP28" s="27"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="18"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="18"/>
+      <c r="AM28" s="18"/>
+      <c r="AN28" s="18"/>
+      <c r="AO28" s="18"/>
+      <c r="AP28" s="18"/>
       <c r="AQ28" s="18"/>
       <c r="AR28" s="18"/>
       <c r="AS28" s="18"/>
@@ -2524,19 +2525,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
+    <row r="29" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="37"/>
       <c r="B29" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
@@ -2544,11 +2545,11 @@
       <c r="O29" s="18"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
       <c r="W29" s="18"/>
       <c r="X29" s="18"/>
       <c r="Y29" s="18"/>
@@ -2557,18 +2558,18 @@
       <c r="AB29" s="18"/>
       <c r="AC29" s="18"/>
       <c r="AD29" s="18"/>
-      <c r="AE29" s="27"/>
-      <c r="AF29" s="27"/>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="27"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27"/>
-      <c r="AK29" s="27"/>
-      <c r="AL29" s="27"/>
-      <c r="AM29" s="27"/>
-      <c r="AN29" s="27"/>
-      <c r="AO29" s="27"/>
-      <c r="AP29" s="27"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="18"/>
       <c r="AQ29" s="18"/>
       <c r="AR29" s="18"/>
       <c r="AS29" s="18"/>
@@ -2584,137 +2585,143 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="18"/>
-      <c r="AA30" s="18"/>
-      <c r="AB30" s="18"/>
-      <c r="AC30" s="18"/>
-      <c r="AD30" s="18"/>
-      <c r="AE30" s="18"/>
-      <c r="AF30" s="18"/>
-      <c r="AG30" s="18"/>
-      <c r="AH30" s="18"/>
-      <c r="AI30" s="18"/>
-      <c r="AJ30" s="18"/>
-      <c r="AK30" s="18"/>
-      <c r="AL30" s="18"/>
-      <c r="AM30" s="18"/>
-      <c r="AN30" s="18"/>
-      <c r="AO30" s="18"/>
-      <c r="AP30" s="18"/>
-      <c r="AQ30" s="18"/>
-      <c r="AR30" s="18"/>
-      <c r="AS30" s="18"/>
-      <c r="AT30" s="18"/>
-      <c r="AU30" s="18"/>
-      <c r="AV30" s="18"/>
-      <c r="AW30" s="20">
+    <row r="30" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="37"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="25"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="25"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="25"/>
+      <c r="X30" s="25"/>
+      <c r="Y30" s="25"/>
+      <c r="Z30" s="25"/>
+      <c r="AA30" s="25"/>
+      <c r="AB30" s="25"/>
+      <c r="AC30" s="25"/>
+      <c r="AD30" s="25"/>
+      <c r="AE30" s="25"/>
+      <c r="AF30" s="25"/>
+      <c r="AG30" s="25"/>
+      <c r="AH30" s="25"/>
+      <c r="AI30" s="25"/>
+      <c r="AJ30" s="25"/>
+      <c r="AK30" s="25"/>
+      <c r="AL30" s="25"/>
+      <c r="AM30" s="25"/>
+      <c r="AN30" s="25"/>
+      <c r="AO30" s="25"/>
+      <c r="AP30" s="25"/>
+      <c r="AQ30" s="25"/>
+      <c r="AR30" s="25"/>
+      <c r="AS30" s="25"/>
+      <c r="AT30" s="25"/>
+      <c r="AU30" s="25"/>
+      <c r="AV30" s="25"/>
+      <c r="AW30" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX30" s="21">
-        <f>IF(AW30&gt;7.5, AW30 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="18"/>
-      <c r="Z31" s="18"/>
-      <c r="AA31" s="18"/>
-      <c r="AB31" s="18"/>
-      <c r="AC31" s="18"/>
-      <c r="AD31" s="18"/>
-      <c r="AE31" s="18"/>
-      <c r="AF31" s="18"/>
-      <c r="AG31" s="18"/>
-      <c r="AH31" s="18"/>
-      <c r="AI31" s="18"/>
-      <c r="AJ31" s="18"/>
-      <c r="AK31" s="18"/>
-      <c r="AL31" s="18"/>
-      <c r="AM31" s="18"/>
-      <c r="AN31" s="18"/>
-      <c r="AO31" s="18"/>
-      <c r="AP31" s="18"/>
-      <c r="AQ31" s="18"/>
-      <c r="AR31" s="18"/>
-      <c r="AS31" s="18"/>
-      <c r="AT31" s="18"/>
-      <c r="AU31" s="18"/>
-      <c r="AV31" s="18"/>
-      <c r="AW31" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX31" s="21">
-        <f>IF(AW31&gt;7.5, AW31 - 7.5, )</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
+      <c r="AX30" s="12">
+        <f>IF(AW30&gt;0, AW30, )</f>
+        <v>0</v>
+      </c>
+      <c r="AY30" s="13"/>
+      <c r="AZ30" s="13"/>
+      <c r="BA30" s="13"/>
+      <c r="BB30" s="13"/>
+      <c r="BC30" s="13"/>
+      <c r="BD30" s="13"/>
+      <c r="BE30" s="13"/>
+      <c r="BF30" s="13"/>
+      <c r="BG30" s="13"/>
+      <c r="BH30" s="13"/>
+      <c r="BI30" s="13"/>
+      <c r="BJ30" s="13"/>
+      <c r="BK30" s="13"/>
+      <c r="BL30" s="13"/>
+    </row>
+    <row r="31" spans="1:64" s="13" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="37"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="25"/>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AA31" s="25"/>
+      <c r="AB31" s="25"/>
+      <c r="AC31" s="25"/>
+      <c r="AD31" s="25"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
+      <c r="AH31" s="25"/>
+      <c r="AI31" s="25"/>
+      <c r="AJ31" s="25"/>
+      <c r="AK31" s="25"/>
+      <c r="AL31" s="25"/>
+      <c r="AM31" s="25"/>
+      <c r="AN31" s="25"/>
+      <c r="AO31" s="25"/>
+      <c r="AP31" s="25"/>
+      <c r="AQ31" s="25"/>
+      <c r="AR31" s="25"/>
+      <c r="AS31" s="25"/>
+      <c r="AT31" s="25"/>
+      <c r="AU31" s="25"/>
+      <c r="AV31" s="25"/>
+      <c r="AW31" s="26"/>
+      <c r="AX31" s="12"/>
+    </row>
+    <row r="32" spans="1:64" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="37"/>
+      <c r="B32" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -2722,11 +2729,11 @@
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27"/>
+      <c r="U32" s="27"/>
+      <c r="V32" s="27"/>
       <c r="W32" s="18"/>
       <c r="X32" s="18"/>
       <c r="Y32" s="18"/>
@@ -2735,20 +2742,20 @@
       <c r="AB32" s="18"/>
       <c r="AC32" s="18"/>
       <c r="AD32" s="18"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="18"/>
-      <c r="AG32" s="18"/>
-      <c r="AH32" s="18"/>
-      <c r="AI32" s="18"/>
-      <c r="AJ32" s="18"/>
-      <c r="AK32" s="18"/>
-      <c r="AL32" s="18"/>
-      <c r="AM32" s="18"/>
-      <c r="AN32" s="18"/>
-      <c r="AO32" s="18"/>
-      <c r="AP32" s="18"/>
-      <c r="AQ32" s="27"/>
-      <c r="AR32" s="27"/>
+      <c r="AE32" s="27"/>
+      <c r="AF32" s="27"/>
+      <c r="AG32" s="27"/>
+      <c r="AH32" s="27"/>
+      <c r="AI32" s="27"/>
+      <c r="AJ32" s="27"/>
+      <c r="AK32" s="27"/>
+      <c r="AL32" s="27"/>
+      <c r="AM32" s="27"/>
+      <c r="AN32" s="27"/>
+      <c r="AO32" s="27"/>
+      <c r="AP32" s="27"/>
+      <c r="AQ32" s="18"/>
+      <c r="AR32" s="18"/>
       <c r="AS32" s="18"/>
       <c r="AT32" s="18"/>
       <c r="AU32" s="18"/>
@@ -2762,281 +2769,571 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="26"/>
-      <c r="AA33" s="26"/>
-      <c r="AB33" s="26"/>
-      <c r="AC33" s="26"/>
-      <c r="AD33" s="26"/>
-      <c r="AE33" s="26"/>
-      <c r="AF33" s="26"/>
-      <c r="AG33" s="26"/>
-      <c r="AH33" s="26"/>
-      <c r="AI33" s="26"/>
-      <c r="AJ33" s="26"/>
-      <c r="AK33" s="26"/>
-      <c r="AL33" s="26"/>
-      <c r="AM33" s="26"/>
-      <c r="AN33" s="26"/>
-      <c r="AO33" s="26"/>
-      <c r="AP33" s="26"/>
-      <c r="AQ33" s="26"/>
-      <c r="AR33" s="26"/>
-      <c r="AS33" s="26"/>
-      <c r="AT33" s="26"/>
-      <c r="AU33" s="26"/>
-      <c r="AV33" s="26"/>
-      <c r="AW33" s="26">
+    <row r="33" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="37"/>
+      <c r="B33" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27"/>
+      <c r="U33" s="27"/>
+      <c r="V33" s="27"/>
+      <c r="W33" s="18"/>
+      <c r="X33" s="18"/>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="18"/>
+      <c r="AA33" s="18"/>
+      <c r="AB33" s="18"/>
+      <c r="AC33" s="18"/>
+      <c r="AD33" s="18"/>
+      <c r="AE33" s="27"/>
+      <c r="AF33" s="27"/>
+      <c r="AG33" s="27"/>
+      <c r="AH33" s="27"/>
+      <c r="AI33" s="27"/>
+      <c r="AJ33" s="27"/>
+      <c r="AK33" s="27"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="27"/>
+      <c r="AO33" s="27"/>
+      <c r="AP33" s="27"/>
+      <c r="AQ33" s="18"/>
+      <c r="AR33" s="18"/>
+      <c r="AS33" s="18"/>
+      <c r="AT33" s="18"/>
+      <c r="AU33" s="18"/>
+      <c r="AV33" s="18"/>
+      <c r="AW33" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AX33" s="12"/>
-      <c r="AY33" s="13"/>
-      <c r="AZ33" s="13"/>
-      <c r="BA33" s="13"/>
-      <c r="BB33" s="13"/>
-      <c r="BC33" s="13"/>
-      <c r="BD33" s="13"/>
-      <c r="BE33" s="13"/>
-      <c r="BF33" s="13"/>
-      <c r="BG33" s="13"/>
-      <c r="BH33" s="13"/>
-      <c r="BI33" s="13"/>
-      <c r="BJ33" s="13"/>
-      <c r="BK33" s="13"/>
-      <c r="BL33" s="13"/>
-    </row>
-    <row r="34" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="AX33" s="21">
+        <f>IF(AW33&gt;7.5, AW33 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="37"/>
+      <c r="B34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="18"/>
+      <c r="X34" s="18"/>
+      <c r="Y34" s="18"/>
+      <c r="Z34" s="18"/>
+      <c r="AA34" s="18"/>
+      <c r="AB34" s="18"/>
+      <c r="AC34" s="18"/>
+      <c r="AD34" s="18"/>
+      <c r="AE34" s="18"/>
+      <c r="AF34" s="18"/>
+      <c r="AG34" s="18"/>
+      <c r="AH34" s="18"/>
+      <c r="AI34" s="18"/>
+      <c r="AJ34" s="18"/>
+      <c r="AK34" s="18"/>
+      <c r="AL34" s="18"/>
+      <c r="AM34" s="18"/>
+      <c r="AN34" s="18"/>
+      <c r="AO34" s="18"/>
+      <c r="AP34" s="18"/>
+      <c r="AQ34" s="18"/>
+      <c r="AR34" s="18"/>
+      <c r="AS34" s="18"/>
+      <c r="AT34" s="18"/>
+      <c r="AU34" s="18"/>
+      <c r="AV34" s="18"/>
+      <c r="AW34" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX34" s="21">
+        <f>IF(AW34&gt;7.5, AW34 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="37"/>
+      <c r="B35" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+      <c r="V35" s="18"/>
+      <c r="W35" s="18"/>
+      <c r="X35" s="18"/>
+      <c r="Y35" s="18"/>
+      <c r="Z35" s="18"/>
+      <c r="AA35" s="18"/>
+      <c r="AB35" s="18"/>
+      <c r="AC35" s="18"/>
+      <c r="AD35" s="18"/>
+      <c r="AE35" s="18"/>
+      <c r="AF35" s="18"/>
+      <c r="AG35" s="18"/>
+      <c r="AH35" s="18"/>
+      <c r="AI35" s="18"/>
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+      <c r="AL35" s="18"/>
+      <c r="AM35" s="18"/>
+      <c r="AN35" s="18"/>
+      <c r="AO35" s="18"/>
+      <c r="AP35" s="18"/>
+      <c r="AQ35" s="18"/>
+      <c r="AR35" s="18"/>
+      <c r="AS35" s="18"/>
+      <c r="AT35" s="18"/>
+      <c r="AU35" s="18"/>
+      <c r="AV35" s="18"/>
+      <c r="AW35" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX35" s="21">
+        <f>IF(AW35&gt;7.5, AW35 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="37"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
+      <c r="U36" s="18"/>
+      <c r="V36" s="18"/>
+      <c r="W36" s="18"/>
+      <c r="X36" s="18"/>
+      <c r="Y36" s="18"/>
+      <c r="Z36" s="18"/>
+      <c r="AA36" s="18"/>
+      <c r="AB36" s="18"/>
+      <c r="AC36" s="18"/>
+      <c r="AD36" s="18"/>
+      <c r="AE36" s="18"/>
+      <c r="AF36" s="18"/>
+      <c r="AG36" s="18"/>
+      <c r="AH36" s="18"/>
+      <c r="AI36" s="18"/>
+      <c r="AJ36" s="18"/>
+      <c r="AK36" s="18"/>
+      <c r="AL36" s="18"/>
+      <c r="AM36" s="18"/>
+      <c r="AN36" s="18"/>
+      <c r="AO36" s="18"/>
+      <c r="AP36" s="18"/>
+      <c r="AQ36" s="27"/>
+      <c r="AR36" s="27"/>
+      <c r="AS36" s="18"/>
+      <c r="AT36" s="18"/>
+      <c r="AU36" s="18"/>
+      <c r="AV36" s="18"/>
+      <c r="AW36" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX36" s="21">
+        <f>IF(AW36&gt;7.5, AW36 - 7.5, )</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:64" s="14" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="37"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="26"/>
+      <c r="X37" s="26"/>
+      <c r="Y37" s="26"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+      <c r="AB37" s="26"/>
+      <c r="AC37" s="26"/>
+      <c r="AD37" s="26"/>
+      <c r="AE37" s="26"/>
+      <c r="AF37" s="26"/>
+      <c r="AG37" s="26"/>
+      <c r="AH37" s="26"/>
+      <c r="AI37" s="26"/>
+      <c r="AJ37" s="26"/>
+      <c r="AK37" s="26"/>
+      <c r="AL37" s="26"/>
+      <c r="AM37" s="26"/>
+      <c r="AN37" s="26"/>
+      <c r="AO37" s="26"/>
+      <c r="AP37" s="26"/>
+      <c r="AQ37" s="26"/>
+      <c r="AR37" s="26"/>
+      <c r="AS37" s="26"/>
+      <c r="AT37" s="26"/>
+      <c r="AU37" s="26"/>
+      <c r="AV37" s="26"/>
+      <c r="AW37" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AX37" s="12"/>
+      <c r="AY37" s="13"/>
+      <c r="AZ37" s="13"/>
+      <c r="BA37" s="13"/>
+      <c r="BB37" s="13"/>
+      <c r="BC37" s="13"/>
+      <c r="BD37" s="13"/>
+      <c r="BE37" s="13"/>
+      <c r="BF37" s="13"/>
+      <c r="BG37" s="13"/>
+      <c r="BH37" s="13"/>
+      <c r="BI37" s="13"/>
+      <c r="BJ37" s="13"/>
+      <c r="BK37" s="13"/>
+      <c r="BL37" s="13"/>
+    </row>
+    <row r="38" spans="1:64" s="13" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="38"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="26"/>
+      <c r="AB38" s="26"/>
+      <c r="AC38" s="26"/>
+      <c r="AD38" s="26"/>
+      <c r="AE38" s="26"/>
+      <c r="AF38" s="26"/>
+      <c r="AG38" s="26"/>
+      <c r="AH38" s="26"/>
+      <c r="AI38" s="26"/>
+      <c r="AJ38" s="26"/>
+      <c r="AK38" s="26"/>
+      <c r="AL38" s="26"/>
+      <c r="AM38" s="26"/>
+      <c r="AN38" s="26"/>
+      <c r="AO38" s="26"/>
+      <c r="AP38" s="26"/>
+      <c r="AQ38" s="26"/>
+      <c r="AR38" s="26"/>
+      <c r="AS38" s="26"/>
+      <c r="AT38" s="26"/>
+      <c r="AU38" s="26"/>
+      <c r="AV38" s="26"/>
+      <c r="AW38" s="26"/>
+      <c r="AX38" s="12"/>
+    </row>
+    <row r="39" spans="1:64" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31">
-        <f t="shared" ref="C34:AX34" si="1">SUM(C4:C33)</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AB34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AD34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AE34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AF34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AG34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AH34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AI34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AM34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AN34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AO34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AP34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AQ34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AR34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AS34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AT34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AU34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV34" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AW34" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AX34" s="33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:64" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="31">
+        <f t="shared" ref="C39:AX39" si="1">SUM(C4:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="X39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AK39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AN39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AO39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AP39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AQ39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AR39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AS39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AT39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AU39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AV39" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AW39" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AX39" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:64" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:A33"/>
+    <mergeCell ref="A3:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>